<commit_message>
final check before submission
</commit_message>
<xml_diff>
--- a/Milestone1/Gantt Chart/GanttChart.xlsx
+++ b/Milestone1/Gantt Chart/GanttChart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sipa/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0e2cabc86ace0c42/Documents/Uni/2810ICT - Software Technologies/2024/Assignment/Group Project/SoftwareTechAssign/Milestone1/Gantt Chart/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED6850FA-2456-094E-979A-130BB215425F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{ED6850FA-2456-094E-979A-130BB215425F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5993EE60-5BA3-4AFC-BD8F-21F5A270E2C0}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1665" yWindow="165" windowWidth="19470" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -639,6 +639,33 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="10" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="12">
       <alignment vertical="center"/>
     </xf>
@@ -650,33 +677,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="10" applyFont="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="10" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1080,23 +1080,23 @@
   </sheetPr>
   <dimension ref="B1:BO39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="82" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="82" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="41.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.625" customWidth="1"/>
+    <col min="2" max="2" width="41.375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="6.625" style="1" customWidth="1"/>
     <col min="4" max="4" width="7" style="1" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="6.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" style="4" customWidth="1"/>
-    <col min="8" max="16" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.375" style="4" customWidth="1"/>
+    <col min="8" max="16" width="3.125" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="27" width="3.5" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="41" width="3.5" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="2.6640625" customWidth="1"/>
+    <col min="42" max="42" width="2.625" customWidth="1"/>
     <col min="43" max="67" width="3.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1110,50 +1110,50 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="2:67" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
+    <row r="2" spans="2:67" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
       <c r="G2" s="21" t="s">
         <v>14</v>
       </c>
       <c r="H2" s="12">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="J2" s="13"/>
-      <c r="K2" s="30" t="s">
+      <c r="K2" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="32"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="28"/>
       <c r="P2" s="14"/>
-      <c r="Q2" s="30" t="s">
+      <c r="Q2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="32"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="28"/>
       <c r="U2" s="15"/>
-      <c r="V2" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="W2" s="35"/>
-      <c r="X2" s="35"/>
-      <c r="Y2" s="36"/>
+      <c r="V2" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" s="31"/>
+      <c r="X2" s="31"/>
+      <c r="Y2" s="32"/>
       <c r="Z2" s="16"/>
-      <c r="AA2" s="34" t="s">
+      <c r="AA2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="AB2" s="35"/>
-      <c r="AC2" s="35"/>
-      <c r="AD2" s="35"/>
-      <c r="AE2" s="35"/>
-      <c r="AF2" s="35"/>
-      <c r="AG2" s="36"/>
+      <c r="AB2" s="31"/>
+      <c r="AC2" s="31"/>
+      <c r="AD2" s="31"/>
+      <c r="AE2" s="31"/>
+      <c r="AF2" s="31"/>
+      <c r="AG2" s="32"/>
       <c r="AH2" s="17"/>
       <c r="AI2" s="19" t="s">
         <v>3</v>
@@ -1166,23 +1166,23 @@
       <c r="AO2" s="20"/>
       <c r="AP2" s="20"/>
     </row>
-    <row r="3" spans="2:67" s="9" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="25" t="s">
+    <row r="3" spans="2:67" s="9" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="29" t="s">
+      <c r="G3" s="24" t="s">
         <v>13</v>
       </c>
       <c r="H3" s="18" t="s">
@@ -1208,13 +1208,13 @@
       <c r="Z3" s="8"/>
       <c r="AA3" s="8"/>
     </row>
-    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="26"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
+    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="35"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
         <v>25</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
         <v>26</v>
       </c>
@@ -1436,7 +1436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
         <v>27</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
         <v>17</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
         <v>18</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
         <v>47</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
         <v>19</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
         <v>20</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="23" t="s">
         <v>21</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="23" t="s">
         <v>22</v>
       </c>
@@ -1592,7 +1592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="23" t="s">
         <v>23</v>
       </c>
@@ -1608,7 +1608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="23" t="s">
         <v>24</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="23" t="s">
         <v>28</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="23" t="s">
         <v>29</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="23" t="s">
         <v>48</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="23" t="s">
         <v>30</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="23" t="s">
         <v>31</v>
       </c>
@@ -1704,7 +1704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="23" t="s">
         <v>32</v>
       </c>
@@ -1720,7 +1720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="23" t="s">
         <v>33</v>
       </c>
@@ -1740,7 +1740,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="23" t="s">
         <v>34</v>
       </c>
@@ -1760,7 +1760,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="23" t="s">
         <v>35</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="23" t="s">
         <v>36</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="23" t="s">
         <v>37</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="23" t="s">
         <v>38</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="23" t="s">
         <v>39</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="23" t="s">
         <v>40</v>
       </c>
@@ -1864,7 +1864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="23" t="s">
         <v>41</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="23" t="s">
         <v>42</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="23" t="s">
         <v>43</v>
       </c>
@@ -1912,7 +1912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="23" t="s">
         <v>44</v>
       </c>
@@ -1928,7 +1928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="23" t="s">
         <v>45</v>
       </c>
@@ -1944,7 +1944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="23" t="s">
         <v>46</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="23" t="s">
         <v>6</v>
       </c>
@@ -1972,7 +1972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="23" t="s">
         <v>7</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="23" t="s">
         <v>8</v>
       </c>
@@ -1998,17 +1998,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA2:AG2"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:BO4">
     <cfRule type="expression" dxfId="8" priority="8">

</xml_diff>

<commit_message>
added all pdfs and missing files for submission
</commit_message>
<xml_diff>
--- a/Milestone1/Gantt Chart/GanttChart.xlsx
+++ b/Milestone1/Gantt Chart/GanttChart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sipa/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0e2cabc86ace0c42/Documents/Uni/2810ICT - Software Technologies/2024/Assignment/Group Project/SoftwareTechAssign/Milestone1/Gantt Chart/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD377ABE-F0E7-4A4D-8C0A-5F120305ED3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="8_{AD377ABE-F0E7-4A4D-8C0A-5F120305ED3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0FFF8DCB-263F-42E4-BE30-E5DF38AFB975}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="6600" windowWidth="28800" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -639,12 +639,24 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="12">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="9" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="10" applyFont="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="10" applyFont="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -665,18 +677,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="12">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="10" applyFont="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1080,24 +1080,24 @@
   </sheetPr>
   <dimension ref="B1:BO39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="68" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="CH30" sqref="CH30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="41.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.625" customWidth="1"/>
+    <col min="2" max="2" width="41.375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="6.625" style="1" customWidth="1"/>
     <col min="4" max="4" width="7" style="1" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="6.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" style="4" customWidth="1"/>
-    <col min="8" max="16" width="2.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="27" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="41" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="2.6640625" customWidth="1"/>
-    <col min="43" max="67" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.375" style="4" customWidth="1"/>
+    <col min="8" max="16" width="2.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="27" width="3.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="41" width="3.125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="2.625" customWidth="1"/>
+    <col min="43" max="67" width="3.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
@@ -1110,50 +1110,50 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="2:67" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+    <row r="2" spans="2:67" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
       <c r="G2" s="21" t="s">
         <v>14</v>
       </c>
       <c r="H2" s="12">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="J2" s="13"/>
-      <c r="K2" s="26" t="s">
+      <c r="K2" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="28"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="32"/>
       <c r="P2" s="14"/>
-      <c r="Q2" s="26" t="s">
+      <c r="Q2" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="29"/>
-      <c r="S2" s="29"/>
-      <c r="T2" s="28"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="32"/>
       <c r="U2" s="15"/>
-      <c r="V2" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="W2" s="31"/>
-      <c r="X2" s="31"/>
-      <c r="Y2" s="32"/>
+      <c r="V2" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" s="35"/>
+      <c r="X2" s="35"/>
+      <c r="Y2" s="36"/>
       <c r="Z2" s="16"/>
-      <c r="AA2" s="30" t="s">
+      <c r="AA2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="AB2" s="31"/>
-      <c r="AC2" s="31"/>
-      <c r="AD2" s="31"/>
-      <c r="AE2" s="31"/>
-      <c r="AF2" s="31"/>
-      <c r="AG2" s="32"/>
+      <c r="AB2" s="35"/>
+      <c r="AC2" s="35"/>
+      <c r="AD2" s="35"/>
+      <c r="AE2" s="35"/>
+      <c r="AF2" s="35"/>
+      <c r="AG2" s="36"/>
       <c r="AH2" s="17"/>
       <c r="AI2" s="19" t="s">
         <v>3</v>
@@ -1166,23 +1166,23 @@
       <c r="AO2" s="20"/>
       <c r="AP2" s="20"/>
     </row>
-    <row r="3" spans="2:67" s="9" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="34" t="s">
+    <row r="3" spans="2:67" s="9" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="E3" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="29" t="s">
         <v>13</v>
       </c>
       <c r="H3" s="18" t="s">
@@ -1208,13 +1208,13 @@
       <c r="Z3" s="8"/>
       <c r="AA3" s="8"/>
     </row>
-    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="35"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
+    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="26"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
         <v>25</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
         <v>26</v>
       </c>
@@ -1433,10 +1433,10 @@
         <v>1</v>
       </c>
       <c r="G6" s="22">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
         <v>27</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
         <v>17</v>
       </c>
@@ -1473,10 +1473,10 @@
         <v>16</v>
       </c>
       <c r="G8" s="22">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
         <v>18</v>
       </c>
@@ -1493,10 +1493,10 @@
         <v>2</v>
       </c>
       <c r="G9" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
         <v>47</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
         <v>19</v>
       </c>
@@ -1533,10 +1533,10 @@
         <v>4</v>
       </c>
       <c r="G11" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
         <v>20</v>
       </c>
@@ -1553,10 +1553,10 @@
         <v>2</v>
       </c>
       <c r="G12" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="23" t="s">
         <v>21</v>
       </c>
@@ -1573,10 +1573,10 @@
         <v>4</v>
       </c>
       <c r="G13" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="23" t="s">
         <v>22</v>
       </c>
@@ -1593,10 +1593,10 @@
         <v>14</v>
       </c>
       <c r="G14" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="23" t="s">
         <v>23</v>
       </c>
@@ -1613,10 +1613,10 @@
         <v>3</v>
       </c>
       <c r="G15" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="23" t="s">
         <v>24</v>
       </c>
@@ -1633,10 +1633,10 @@
         <v>2</v>
       </c>
       <c r="G16" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="23" t="s">
         <v>28</v>
       </c>
@@ -1653,10 +1653,10 @@
         <v>3</v>
       </c>
       <c r="G17" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="23" t="s">
         <v>29</v>
       </c>
@@ -1673,10 +1673,10 @@
         <v>3</v>
       </c>
       <c r="G18" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="23" t="s">
         <v>48</v>
       </c>
@@ -1693,10 +1693,10 @@
         <v>7</v>
       </c>
       <c r="G19" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="23" t="s">
         <v>30</v>
       </c>
@@ -1713,10 +1713,10 @@
         <v>6</v>
       </c>
       <c r="G20" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="23" t="s">
         <v>31</v>
       </c>
@@ -1733,10 +1733,10 @@
         <v>3</v>
       </c>
       <c r="G21" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="23" t="s">
         <v>32</v>
       </c>
@@ -1753,10 +1753,10 @@
         <v>3</v>
       </c>
       <c r="G22" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="23" t="s">
         <v>33</v>
       </c>
@@ -1773,10 +1773,10 @@
         <v>44</v>
       </c>
       <c r="G23" s="22">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="23" t="s">
         <v>34</v>
       </c>
@@ -1793,10 +1793,10 @@
         <v>44</v>
       </c>
       <c r="G24" s="22">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="23" t="s">
         <v>35</v>
       </c>
@@ -1813,10 +1813,10 @@
         <v>44</v>
       </c>
       <c r="G25" s="22">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="23" t="s">
         <v>36</v>
       </c>
@@ -1833,10 +1833,10 @@
         <v>44</v>
       </c>
       <c r="G26" s="22">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="23" t="s">
         <v>37</v>
       </c>
@@ -1853,10 +1853,10 @@
         <v>27</v>
       </c>
       <c r="G27" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="23" t="s">
         <v>38</v>
       </c>
@@ -1873,10 +1873,10 @@
         <v>27</v>
       </c>
       <c r="G28" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="23" t="s">
         <v>39</v>
       </c>
@@ -1893,10 +1893,10 @@
         <v>27</v>
       </c>
       <c r="G29" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="23" t="s">
         <v>40</v>
       </c>
@@ -1913,10 +1913,10 @@
         <v>27</v>
       </c>
       <c r="G30" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="23" t="s">
         <v>41</v>
       </c>
@@ -1933,10 +1933,10 @@
         <v>20</v>
       </c>
       <c r="G31" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="23" t="s">
         <v>42</v>
       </c>
@@ -1953,10 +1953,10 @@
         <v>20</v>
       </c>
       <c r="G32" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="23" t="s">
         <v>43</v>
       </c>
@@ -1973,10 +1973,10 @@
         <v>7</v>
       </c>
       <c r="G33" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="23" t="s">
         <v>44</v>
       </c>
@@ -1993,10 +1993,10 @@
         <v>7</v>
       </c>
       <c r="G34" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="23" t="s">
         <v>45</v>
       </c>
@@ -2013,10 +2013,10 @@
         <v>1</v>
       </c>
       <c r="G35" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="23" t="s">
         <v>46</v>
       </c>
@@ -2033,10 +2033,10 @@
         <v>1</v>
       </c>
       <c r="G36" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="23" t="s">
         <v>6</v>
       </c>
@@ -2048,7 +2048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="23" t="s">
         <v>7</v>
       </c>
@@ -2060,7 +2060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="23" t="s">
         <v>8</v>
       </c>
@@ -2074,17 +2074,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA2:AG2"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:BO4">
     <cfRule type="expression" dxfId="8" priority="8">

</xml_diff>